<commit_message>
Modificación de archivos product_import
</commit_message>
<xml_diff>
--- a/humanidades/products_import_final.xlsx
+++ b/humanidades/products_import_final.xlsx
@@ -232,7 +232,7 @@
     <t xml:space="preserve">275.5</t>
   </si>
   <si>
-    <t xml:space="preserve">http://demo-tienda.acatlan.unam.mx//Libreria-FES-ACATLAN/humanidades/img/lecturas_selectas_de_historiografia_linguistica_ii.jpg</t>
+    <t xml:space="preserve">http://132.248.80.70/prestashop/Libreria-FES-ACATLAN/humanidades/img/lecturas_selectas_de_historiografia_linguistica_ii.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">lecturas-selectas-historiografia</t>
@@ -253,7 +253,7 @@
     <t xml:space="preserve">118.5</t>
   </si>
   <si>
-    <t xml:space="preserve">http://demo-tienda.acatlan.unam.mx//Libreria-FES-ACATLAN/humanidades/img/arquitectura_romanica.jpg</t>
+    <t xml:space="preserve">http://132.248.80.70/prestashop/Libreria-FES-ACATLAN/humanidades/img/arquitectura_romanica.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">arquitectura-romanica</t>
@@ -274,7 +274,7 @@
     <t xml:space="preserve">195.5</t>
   </si>
   <si>
-    <t xml:space="preserve">http://demo-tienda.acatlan.unam.mx//Libreria-FES-ACATLAN/humanidades/img/la_educacion_jesuita_en_la_nueva_españa.jpg</t>
+    <t xml:space="preserve">http://132.248.80.70/prestashop/Libreria-FES-ACATLAN/humanidades/img/la_educacion_jesuita_en_la_nueva_españa.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">educacion-jesuita-nueva-españa</t>
@@ -289,7 +289,7 @@
     <t xml:space="preserve">21.5</t>
   </si>
   <si>
-    <t xml:space="preserve">http://demo-tienda.acatlan.unam.mx//Libreria-FES-ACATLAN/humanidades/img/historia_del_nacionalismo_occitano_en_francia.jpg</t>
+    <t xml:space="preserve">http://132.248.80.70/prestashop/Libreria-FES-ACATLAN/humanidades/img/historia_del_nacionalismo_occitano_en_francia.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">historia-nacionalismo-occitano</t>
@@ -310,7 +310,7 @@
     <t xml:space="preserve">0.7</t>
   </si>
   <si>
-    <t xml:space="preserve">http://demo-tienda.acatlan.unam.mx//Libreria-FES-ACATLAN/humanidades/img/una_experiencia_innovadora.jpg</t>
+    <t xml:space="preserve">http://132.248.80.70/prestashop/Libreria-FES-ACATLAN/humanidades/img/una_experiencia_innovadora.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">experiencia-innovadora</t>
@@ -354,7 +354,7 @@
     <t xml:space="preserve">1.9</t>
   </si>
   <si>
-    <t xml:space="preserve">http://demo-tienda.acatlan.unam.mx//Libreria-FES-ACATLAN/humanidades/img/clasicos_de_la_pedagogia.jpg</t>
+    <t xml:space="preserve">http://132.248.80.70/prestashop/Libreria-FES-ACATLAN/humanidades/img/clasicos_de_la_pedagogia.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">clasicos-pedagogia</t>
@@ -375,7 +375,7 @@
     <t xml:space="preserve">425.5</t>
   </si>
   <si>
-    <t xml:space="preserve">http://demo-tienda.acatlan.unam.mx//Libreria-FES-ACATLAN/humanidades/img/historia_del_arte_i.jpg</t>
+    <t xml:space="preserve">http://132.248.80.70/prestashop/Libreria-FES-ACATLAN/humanidades/img/historia_del_arte_i.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">historia-arte</t>
@@ -390,7 +390,7 @@
     <t xml:space="preserve">424.5</t>
   </si>
   <si>
-    <t xml:space="preserve">http://demo-tienda.acatlan.unam.mx//Libreria-FES-ACATLAN/humanidades/img/historia_del_arte_ii.jpg</t>
+    <t xml:space="preserve">http://132.248.80.70/prestashop/Libreria-FES-ACATLAN/humanidades/img/historia_del_arte_ii.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Autor:Adria Paulina Milagros Pichardo Hernández:1,Primera Edición 2013:2,Páginas:267:3</t>
@@ -399,7 +399,7 @@
     <t xml:space="preserve">El barroco hecho discurso: Retórica de un sermón novohispano del siglo XVII</t>
   </si>
   <si>
-    <t xml:space="preserve">http://demo-tienda.acatlan.unam.mx//Libreria-FES-ACATLAN/humanidades/img/el_barroco_hecho_discurso.jpg</t>
+    <t xml:space="preserve">http://132.248.80.70/prestashop/Libreria-FES-ACATLAN/humanidades/img/el_barroco_hecho_discurso.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">barroco-hecho-discurso</t>
@@ -418,7 +418,7 @@
     <t xml:space="preserve">0.4</t>
   </si>
   <si>
-    <t xml:space="preserve">http://demo-tienda.acatlan.unam.mx//Libreria-FES-ACATLAN/humanidades/img/el_templo_en_la_arquitectura_griega.jpg</t>
+    <t xml:space="preserve">http://132.248.80.70/prestashop/Libreria-FES-ACATLAN/humanidades/img/el_templo_en_la_arquitectura_griega.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">templo-arquitectura-griega</t>
@@ -433,7 +433,7 @@
     <t xml:space="preserve">16.7</t>
   </si>
   <si>
-    <t xml:space="preserve">http://demo-tienda.acatlan.unam.mx//Libreria-FES-ACATLAN/humanidades/img/obras_de_juan_a_ortega_y_medina_europa_moderna_1.jpg</t>
+    <t xml:space="preserve">http://132.248.80.70/prestashop/Libreria-FES-ACATLAN/humanidades/img/obras_de_juan_a_ortega_y_medina_europa_moderna_1.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">ortega-europa-moderna</t>
@@ -474,7 +474,7 @@
     <t xml:space="preserve">1254.5</t>
   </si>
   <si>
-    <t xml:space="preserve">http://demo-tienda.acatlan.unam.mx//Libreria-FES-ACATLAN/humanidades/img/obras_de_juan_a_ortega_y_medina_evangelizacion_y_destino.jpg</t>
+    <t xml:space="preserve">http://132.248.80.70/prestashop/Libreria-FES-ACATLAN/humanidades/img/obras_de_juan_a_ortega_y_medina_evangelizacion_y_destino.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">ortega-evangelizaicon-destino</t>
@@ -489,7 +489,7 @@
     <t xml:space="preserve">372.5</t>
   </si>
   <si>
-    <t xml:space="preserve">http://demo-tienda.acatlan.unam.mx//Libreria-FES-ACATLAN/humanidades/img/la_diplomacia_municipal_en_mexico_cinco_estudios_de_caso.jpg</t>
+    <t xml:space="preserve">http://132.248.80.70/prestashop/Libreria-FES-ACATLAN/humanidades/img/la_diplomacia_municipal_en_mexico_cinco_estudios_de_caso.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">diplomacia-municipal-mexico</t>
@@ -504,7 +504,7 @@
     <t xml:space="preserve">1.8</t>
   </si>
   <si>
-    <t xml:space="preserve">http://demo-tienda.acatlan.unam.mx//Libreria-FES-ACATLAN/humanidades/img/paginas_de_la_hoja_volandera_1.jpg</t>
+    <t xml:space="preserve">http://132.248.80.70/prestashop/Libreria-FES-ACATLAN/humanidades/img/paginas_de_la_hoja_volandera_1.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">hoja-volandera</t>
@@ -516,7 +516,7 @@
     <t xml:space="preserve">Páginas de la Hoja Volandera 2</t>
   </si>
   <si>
-    <t xml:space="preserve">http://demo-tienda.acatlan.unam.mx//Libreria-FES-ACATLAN/humanidades/img/paginas_de_la_hoja_volandera_2.jpg</t>
+    <t xml:space="preserve">http://132.248.80.70/prestashop/Libreria-FES-ACATLAN/humanidades/img/paginas_de_la_hoja_volandera_2.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Compilador:Sergio Montes García:1,Primera Edición 2014:2,Páginas:363:3</t>
@@ -534,7 +534,7 @@
     <t xml:space="preserve">477.5</t>
   </si>
   <si>
-    <t xml:space="preserve">http://132.248.80.70/tienda/Libreria-FES-ACATLAN/humanidades/img/de_literatura_e_historia_de_mexico.jpg</t>
+    <t xml:space="preserve">http://132.248.80.70/prestashop/Libreria-FES-ACATLAN/humanidades/img/de_literatura_e_historia_de_mexico.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">literatura-historia-mexico</t>
@@ -558,7 +558,7 @@
     <t xml:space="preserve">310.5</t>
   </si>
   <si>
-    <t xml:space="preserve">http://132.248.80.70/tienda/Libreria-FES-ACATLAN/humanidades/img/las_generaciones_de_la_poesia_del_renacimiento_español_y_novohispano_una_propuesta.jpg</t>
+    <t xml:space="preserve">http://132.248.80.70/prestashop/Libreria-FES-ACATLAN/humanidades/img/las_generaciones_de_la_poesia_del_renacimiento_español_y_novohispano_una_propuesta.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">poesia-renacimiento-español</t>
@@ -576,7 +576,7 @@
     <t xml:space="preserve">1000.5</t>
   </si>
   <si>
-    <t xml:space="preserve">http://132.248.80.70/tienda/Libreria-FES-ACATLAN/humanidades/img/obras_de_juan_a_ortega_y_medina_literatura_viajera.jpg</t>
+    <t xml:space="preserve">http://132.248.80.70/prestashop/Libreria-FES-ACATLAN/humanidades/img/obras_de_juan_a_ortega_y_medina_literatura_viajera.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">ortega-literatura-viajera</t>
@@ -594,7 +594,7 @@
     <t xml:space="preserve">134.</t>
   </si>
   <si>
-    <t xml:space="preserve">http://132.248.80.70/tienda/Libreria-FES-ACATLAN/humanidades/img/la_alfabetizacion_informal_en_el_siglo_xxi.jpg</t>
+    <t xml:space="preserve">http://132.248.80.70/prestashop/Libreria-FES-ACATLAN/humanidades/img/la_alfabetizacion_informal_en_el_siglo_xxi.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">alfabetizacion-informal-siglo</t>
@@ -615,7 +615,7 @@
     <t xml:space="preserve">626.5</t>
   </si>
   <si>
-    <t xml:space="preserve">http://132.248.80.70/tienda/Libreria-FES-ACATLAN/humanidades/img/obras_de_juan_a_ortega_y_medina_humboldt.jpg</t>
+    <t xml:space="preserve">http://132.248.80.70/prestashop/Libreria-FES-ACATLAN/humanidades/img/obras_de_juan_a_ortega_y_medina_humboldt.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">ortega-humboldt</t>
@@ -630,7 +630,7 @@
     <t xml:space="preserve">2.5</t>
   </si>
   <si>
-    <t xml:space="preserve">http://132.248.80.70/tienda/Libreria-FES-ACATLAN/humanidades/img/obras_de_juan_a_ortega_y_medina_descubrimiento_y_conquista.jpg</t>
+    <t xml:space="preserve">http://132.248.80.70/prestashop/Libreria-FES-ACATLAN/humanidades/img/obras_de_juan_a_ortega_y_medina_descubrimiento_y_conquista.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">ortega-descubrimiento-conquista</t>
@@ -645,7 +645,7 @@
     <t xml:space="preserve">230.5</t>
   </si>
   <si>
-    <t xml:space="preserve">http://132.248.80.70/tienda/Libreria-FES-ACATLAN/humanidades/img/las_bases_de_la_modernidad_john_locke.jpg</t>
+    <t xml:space="preserve">http://132.248.80.70/prestashop/Libreria-FES-ACATLAN/humanidades/img/las_bases_de_la_modernidad_john_locke.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">bases-modernidad-locke</t>
@@ -669,7 +669,7 @@
     <t xml:space="preserve">91.5</t>
   </si>
   <si>
-    <t xml:space="preserve">http://132.248.80.70/tienda/Libreria-FES-ACATLAN/humanidades/img/cultura_paradigmas_y_significados.jpg</t>
+    <t xml:space="preserve">http://132.248.80.70/prestashop/Libreria-FES-ACATLAN/humanidades/img/cultura_paradigmas_y_significados.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">cultura-paradigmas-significados</t>
@@ -684,7 +684,7 @@
     <t xml:space="preserve">478.5</t>
   </si>
   <si>
-    <t xml:space="preserve">http://132.248.80.70/tienda/Libreria-FES-ACATLAN/humanidades/img/de_educacion_y_otros_temas.jpg</t>
+    <t xml:space="preserve">http://132.248.80.70/prestashop/Libreria-FES-ACATLAN/humanidades/img/de_educacion_y_otros_temas.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">educacion-temas</t>
@@ -702,7 +702,7 @@
     <t xml:space="preserve">22.7</t>
   </si>
   <si>
-    <t xml:space="preserve">http://132.248.80.70/tienda/Libreria-FES-ACATLAN/humanidades/img/de_los_dioses_y_sus_atributos.jpg</t>
+    <t xml:space="preserve">http://132.248.80.70/prestashop/Libreria-FES-ACATLAN/humanidades/img/de_los_dioses_y_sus_atributos.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">dioses-atributos</t>
@@ -717,7 +717,7 @@
     <t xml:space="preserve">15.2</t>
   </si>
   <si>
-    <t xml:space="preserve">http://132.248.80.70/tienda/Libreria-FES-ACATLAN/humanidades/img/las_tecnologias_de_la_informacion_y_la_comunicacion.jpg</t>
+    <t xml:space="preserve">http://132.248.80.70/prestashop/Libreria-FES-ACATLAN/humanidades/img/las_tecnologias_de_la_informacion_y_la_comunicacion.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">tecnologias-informacion-comunicación</t>
@@ -732,7 +732,7 @@
     <t xml:space="preserve">27.5</t>
   </si>
   <si>
-    <t xml:space="preserve">http://132.248.80.70/tienda/Libreria-FES-ACATLAN/humanidades/img/por_una_didactica_para_la_docencia_universitaria.jpg</t>
+    <t xml:space="preserve">http://132.248.80.70/prestashop/Libreria-FES-ACATLAN/humanidades/img/por_una_didactica_para_la_docencia_universitaria.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">didactica-docencia-universitaria</t>
@@ -744,7 +744,7 @@
     <t xml:space="preserve">La entrevista de prensa</t>
   </si>
   <si>
-    <t xml:space="preserve">http://132.248.80.70/tienda/Libreria-FES-ACATLAN/humanidades/img/la_entrevista_de_prensa.jpg</t>
+    <t xml:space="preserve">http://132.248.80.70/prestashop/Libreria-FES-ACATLAN/humanidades/img/la_entrevista_de_prensa.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">entrevista-prensa</t>
@@ -757,7 +757,7 @@
     <t xml:space="preserve">Sociología y Pedagogía Defender la Universidad</t>
   </si>
   <si>
-    <t xml:space="preserve">http://132.248.80.70/tienda/Libreria-FES-ACATLAN/humanidades/img/sociologia_y_pedagogia_defender_la_universidad.jpg</t>
+    <t xml:space="preserve">http://132.248.80.70/prestashop/Libreria-FES-ACATLAN/humanidades/img/sociologia_y_pedagogia_defender_la_universidad.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">sociologia-pedagogia-defender</t>
@@ -771,15 +771,15 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
   <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -864,7 +864,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -879,14 +879,6 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -912,8 +904,8 @@
   </sheetPr>
   <dimension ref="A1:BN30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2:E30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AX1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AX2" activeCellId="0" sqref="AX2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -930,7 +922,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="24.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="22.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="11.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="17.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="17.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="21.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="12.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="14.21"/>
@@ -943,12 +935,12 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="24" style="0" width="8.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="14.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="14.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="29" style="0" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="29" style="0" width="8.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="20.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="5.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="9.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="34" style="0" width="18.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="0" width="15.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="0" width="15.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="24.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="0" width="29.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="0" width="30.33"/>
@@ -971,7 +963,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="56" min="56" style="0" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="62" min="57" style="0" width="16.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="63" min="63" style="0" width="25.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="64" style="0" width="16.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="64" style="0" width="16.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="65" min="65" style="0" width="10.6"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="66" style="0" width="11.52"/>
   </cols>
@@ -1176,7 +1168,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="50.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
@@ -1189,9 +1181,7 @@
       <c r="D2" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E2" s="1"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
+      <c r="G2" s="1"/>
       <c r="Q2" s="0" t="n">
         <v>9786070235467</v>
       </c>
@@ -1207,18 +1197,8 @@
       <c r="W2" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="X2" s="1"/>
-      <c r="Y2" s="1"/>
-      <c r="Z2" s="0" t="n">
-        <v>15</v>
-      </c>
       <c r="AG2" s="1"/>
-      <c r="AR2" s="4"/>
-      <c r="AS2" s="4"/>
-      <c r="AT2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AU2" s="5" t="s">
+      <c r="AU2" s="1" t="s">
         <v>70</v>
       </c>
       <c r="AV2" s="1" t="s">
@@ -1228,7 +1208,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="50.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
@@ -1241,11 +1221,9 @@
       <c r="D3" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E3" s="1" t="n">
+      <c r="G3" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
       <c r="Q3" s="0" t="n">
         <v>9786070234620</v>
       </c>
@@ -1261,20 +1239,10 @@
       <c r="W3" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="X3" s="1"/>
-      <c r="Y3" s="1"/>
-      <c r="Z3" s="0" t="n">
-        <v>15</v>
-      </c>
       <c r="AG3" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="AR3" s="4"/>
-      <c r="AS3" s="4"/>
-      <c r="AT3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AU3" s="5" t="s">
+      <c r="AU3" s="1" t="s">
         <v>77</v>
       </c>
       <c r="AV3" s="1" t="s">
@@ -1284,7 +1252,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="38.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
         <v>3</v>
       </c>
@@ -1297,9 +1265,7 @@
       <c r="D4" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E4" s="1"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
+      <c r="G4" s="1"/>
       <c r="Q4" s="0" t="n">
         <v>97860227455</v>
       </c>
@@ -1315,18 +1281,8 @@
       <c r="W4" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="X4" s="1"/>
-      <c r="Y4" s="1"/>
-      <c r="Z4" s="0" t="n">
-        <v>15</v>
-      </c>
       <c r="AG4" s="1"/>
-      <c r="AR4" s="4"/>
-      <c r="AS4" s="4"/>
-      <c r="AT4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AU4" s="5" t="s">
+      <c r="AU4" s="1" t="s">
         <v>84</v>
       </c>
       <c r="AV4" s="1" t="s">
@@ -1336,7 +1292,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="62.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
         <v>4</v>
       </c>
@@ -1349,11 +1305,9 @@
       <c r="D5" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E5" s="1" t="n">
+      <c r="G5" s="1" t="n">
         <v>200</v>
       </c>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
       <c r="Q5" s="0" t="n">
         <v>9786070240508</v>
       </c>
@@ -1369,20 +1323,10 @@
       <c r="W5" s="1" t="n">
         <v>291</v>
       </c>
-      <c r="X5" s="1"/>
-      <c r="Y5" s="1"/>
-      <c r="Z5" s="0" t="n">
-        <v>15</v>
-      </c>
       <c r="AG5" s="1" t="n">
         <v>200</v>
       </c>
-      <c r="AR5" s="4"/>
-      <c r="AS5" s="4"/>
-      <c r="AT5" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AU5" s="5" t="s">
+      <c r="AU5" s="1" t="s">
         <v>89</v>
       </c>
       <c r="AV5" s="1" t="s">
@@ -1392,7 +1336,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="71.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="88.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
         <v>5</v>
       </c>
@@ -1405,11 +1349,9 @@
       <c r="D6" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E6" s="1" t="n">
+      <c r="G6" s="1" t="n">
         <v>240</v>
       </c>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
       <c r="Q6" s="0" t="n">
         <v>9786070233685</v>
       </c>
@@ -1425,20 +1367,10 @@
       <c r="W6" s="1" t="n">
         <v>225</v>
       </c>
-      <c r="X6" s="1"/>
-      <c r="Y6" s="1"/>
-      <c r="Z6" s="0" t="n">
-        <v>15</v>
-      </c>
       <c r="AG6" s="1" t="n">
         <v>240</v>
       </c>
-      <c r="AR6" s="4"/>
-      <c r="AS6" s="4"/>
-      <c r="AT6" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AU6" s="5" t="s">
+      <c r="AU6" s="1" t="s">
         <v>96</v>
       </c>
       <c r="AV6" s="1" t="s">
@@ -1448,7 +1380,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="50.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
         <v>6</v>
       </c>
@@ -1461,9 +1393,7 @@
       <c r="D7" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E7" s="1"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
+      <c r="G7" s="1"/>
       <c r="Q7" s="0" t="n">
         <v>9789703205516</v>
       </c>
@@ -1479,18 +1409,8 @@
       <c r="W7" s="1" t="n">
         <v>500</v>
       </c>
-      <c r="X7" s="1"/>
-      <c r="Y7" s="1"/>
-      <c r="Z7" s="0" t="n">
-        <v>15</v>
-      </c>
       <c r="AG7" s="1"/>
-      <c r="AR7" s="4"/>
-      <c r="AS7" s="4"/>
-      <c r="AT7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AU7" s="5" t="s">
+      <c r="AU7" s="1" t="s">
         <v>102</v>
       </c>
       <c r="AV7" s="1" t="s">
@@ -1500,7 +1420,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="62.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
         <v>7</v>
       </c>
@@ -1513,9 +1433,7 @@
       <c r="D8" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E8" s="1"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
+      <c r="G8" s="1"/>
       <c r="Q8" s="0" t="n">
         <v>9786070241895</v>
       </c>
@@ -1531,18 +1449,8 @@
       <c r="W8" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="X8" s="1"/>
-      <c r="Y8" s="1"/>
-      <c r="Z8" s="0" t="n">
-        <v>15</v>
-      </c>
       <c r="AG8" s="1"/>
-      <c r="AR8" s="4"/>
-      <c r="AS8" s="4"/>
-      <c r="AT8" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AU8" s="5" t="s">
+      <c r="AU8" s="1" t="s">
         <v>109</v>
       </c>
       <c r="AV8" s="1" t="s">
@@ -1552,7 +1460,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="62.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
         <v>8</v>
       </c>
@@ -1565,7 +1473,7 @@
       <c r="D9" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E9" s="1"/>
+      <c r="G9" s="1"/>
       <c r="Q9" s="0" t="n">
         <v>9786070245343</v>
       </c>
@@ -1581,16 +1489,8 @@
       <c r="W9" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="X9" s="1"/>
-      <c r="Y9" s="1"/>
-      <c r="Z9" s="0" t="n">
-        <v>15</v>
-      </c>
       <c r="AG9" s="1"/>
-      <c r="AT9" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AU9" s="5" t="s">
+      <c r="AU9" s="1" t="s">
         <v>114</v>
       </c>
       <c r="AV9" s="1" t="s">
@@ -1600,7 +1500,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="50.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
         <v>9</v>
       </c>
@@ -1613,7 +1513,7 @@
       <c r="D10" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E10" s="1" t="n">
+      <c r="G10" s="1" t="n">
         <v>320</v>
       </c>
       <c r="Q10" s="0" t="n">
@@ -1631,18 +1531,10 @@
       <c r="W10" s="1" t="n">
         <v>258</v>
       </c>
-      <c r="X10" s="1"/>
-      <c r="Y10" s="1"/>
-      <c r="Z10" s="0" t="n">
-        <v>15</v>
-      </c>
       <c r="AG10" s="1" t="n">
         <v>320</v>
       </c>
-      <c r="AT10" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AU10" s="5" t="s">
+      <c r="AU10" s="1" t="s">
         <v>117</v>
       </c>
       <c r="AV10" s="1" t="s">
@@ -1652,7 +1544,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
         <v>11</v>
       </c>
@@ -1665,7 +1557,7 @@
       <c r="D11" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E11" s="1"/>
+      <c r="G11" s="1"/>
       <c r="Q11" s="0" t="n">
         <v>9786070241345</v>
       </c>
@@ -1681,16 +1573,8 @@
       <c r="W11" s="1" t="n">
         <v>75</v>
       </c>
-      <c r="X11" s="1"/>
-      <c r="Y11" s="1"/>
-      <c r="Z11" s="0" t="n">
-        <v>15</v>
-      </c>
       <c r="AG11" s="1"/>
-      <c r="AT11" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AU11" s="5" t="s">
+      <c r="AU11" s="1" t="s">
         <v>123</v>
       </c>
       <c r="AV11" s="1" t="s">
@@ -1700,7 +1584,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="52.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
         <v>12</v>
       </c>
@@ -1713,7 +1597,7 @@
       <c r="D12" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E12" s="1" t="n">
+      <c r="G12" s="1" t="n">
         <v>240</v>
       </c>
       <c r="Q12" s="0" t="n">
@@ -1731,18 +1615,10 @@
       <c r="W12" s="1" t="n">
         <v>907</v>
       </c>
-      <c r="X12" s="1"/>
-      <c r="Y12" s="1"/>
-      <c r="Z12" s="0" t="n">
-        <v>15</v>
-      </c>
       <c r="AG12" s="1" t="n">
         <v>240</v>
       </c>
-      <c r="AT12" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AU12" s="5" t="s">
+      <c r="AU12" s="1" t="s">
         <v>128</v>
       </c>
       <c r="AV12" s="1" t="s">
@@ -1752,7 +1628,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="50.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
         <v>13</v>
       </c>
@@ -1765,7 +1641,7 @@
       <c r="D13" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E13" s="1"/>
+      <c r="G13" s="1"/>
       <c r="Q13" s="0" t="n">
         <v>9786070248146</v>
       </c>
@@ -1781,16 +1657,8 @@
       <c r="W13" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="X13" s="1"/>
-      <c r="Y13" s="1"/>
-      <c r="Z13" s="0" t="n">
-        <v>15</v>
-      </c>
       <c r="AG13" s="1"/>
-      <c r="AT13" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AU13" s="5" t="s">
+      <c r="AU13" s="1" t="s">
         <v>133</v>
       </c>
       <c r="AV13" s="1" t="s">
@@ -1800,7 +1668,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="50.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
         <v>14</v>
       </c>
@@ -1813,7 +1681,7 @@
       <c r="D14" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E14" s="1" t="n">
+      <c r="G14" s="1" t="n">
         <v>220</v>
       </c>
       <c r="Q14" s="0" t="n">
@@ -1831,18 +1699,10 @@
       <c r="W14" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="X14" s="1"/>
-      <c r="Y14" s="1"/>
-      <c r="Z14" s="0" t="n">
-        <v>15</v>
-      </c>
       <c r="AG14" s="1" t="n">
         <v>220</v>
       </c>
-      <c r="AT14" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AU14" s="5" t="s">
+      <c r="AU14" s="1" t="s">
         <v>138</v>
       </c>
       <c r="AV14" s="1" t="s">
@@ -1852,7 +1712,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="50.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
         <v>15</v>
       </c>
@@ -1865,7 +1725,7 @@
       <c r="D15" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E15" s="1" t="n">
+      <c r="G15" s="1" t="n">
         <v>220</v>
       </c>
       <c r="Q15" s="0" t="n">
@@ -1883,18 +1743,10 @@
       <c r="W15" s="1" t="n">
         <v>536</v>
       </c>
-      <c r="X15" s="1"/>
-      <c r="Y15" s="1"/>
-      <c r="Z15" s="0" t="n">
-        <v>15</v>
-      </c>
       <c r="AG15" s="1" t="n">
         <v>220</v>
       </c>
-      <c r="AT15" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AU15" s="5" t="s">
+      <c r="AU15" s="1" t="s">
         <v>143</v>
       </c>
       <c r="AV15" s="1" t="s">
@@ -1904,7 +1756,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="50.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
         <v>16</v>
       </c>
@@ -1917,7 +1769,7 @@
       <c r="D16" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E16" s="1" t="n">
+      <c r="G16" s="1" t="n">
         <v>220</v>
       </c>
       <c r="Q16" s="0" t="n">
@@ -1935,18 +1787,10 @@
       <c r="W16" s="1" t="n">
         <v>563</v>
       </c>
-      <c r="X16" s="1"/>
-      <c r="Y16" s="1"/>
-      <c r="Z16" s="0" t="n">
-        <v>15</v>
-      </c>
       <c r="AG16" s="1" t="n">
         <v>220</v>
       </c>
-      <c r="AT16" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AU16" s="5" t="s">
+      <c r="AU16" s="1" t="s">
         <v>147</v>
       </c>
       <c r="AV16" s="1" t="s">
@@ -1956,7 +1800,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="50.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
         <v>17</v>
       </c>
@@ -1969,7 +1813,7 @@
       <c r="D17" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E17" s="1"/>
+      <c r="G17" s="1"/>
       <c r="Q17" s="0" t="n">
         <v>9786070257865</v>
       </c>
@@ -1985,16 +1829,8 @@
       <c r="W17" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="X17" s="1"/>
-      <c r="Y17" s="1"/>
-      <c r="Z17" s="0" t="n">
-        <v>15</v>
-      </c>
       <c r="AG17" s="1"/>
-      <c r="AT17" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AU17" s="5" t="s">
+      <c r="AU17" s="1" t="s">
         <v>153</v>
       </c>
       <c r="AV17" s="1" t="s">
@@ -2004,7 +1840,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="38.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
         <v>18</v>
       </c>
@@ -2017,7 +1853,7 @@
       <c r="D18" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E18" s="1" t="n">
+      <c r="G18" s="1" t="n">
         <v>180</v>
       </c>
       <c r="Q18" s="0" t="n">
@@ -2035,18 +1871,10 @@
       <c r="W18" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="X18" s="1"/>
-      <c r="Y18" s="1"/>
-      <c r="Z18" s="0" t="n">
-        <v>15</v>
-      </c>
       <c r="AG18" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="AT18" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AU18" s="5" t="s">
+      <c r="AU18" s="1" t="s">
         <v>161</v>
       </c>
       <c r="AV18" s="1" t="s">
@@ -2056,7 +1884,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="50.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
         <v>19</v>
       </c>
@@ -2069,7 +1897,7 @@
       <c r="D19" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E19" s="1" t="n">
+      <c r="G19" s="1" t="n">
         <v>450</v>
       </c>
       <c r="Q19" s="0" t="n">
@@ -2087,18 +1915,10 @@
       <c r="W19" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="X19" s="1"/>
-      <c r="Y19" s="1"/>
-      <c r="Z19" s="0" t="n">
-        <v>15</v>
-      </c>
       <c r="AG19" s="1" t="n">
         <v>450</v>
       </c>
-      <c r="AT19" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AU19" s="5" t="s">
+      <c r="AU19" s="1" t="s">
         <v>167</v>
       </c>
       <c r="AV19" s="1" t="s">
@@ -2108,20 +1928,20 @@
         <v>169</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="55.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="56.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
         <v>20</v>
       </c>
       <c r="B20" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="4" t="s">
         <v>170</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E20" s="1"/>
+      <c r="G20" s="1"/>
       <c r="Q20" s="0" t="n">
         <v>9786070268809</v>
       </c>
@@ -2137,26 +1957,18 @@
       <c r="W20" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="X20" s="1"/>
-      <c r="Y20" s="1"/>
-      <c r="Z20" s="0" t="n">
-        <v>15</v>
-      </c>
       <c r="AG20" s="1"/>
-      <c r="AT20" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AU20" s="5" t="s">
+      <c r="AU20" s="1" t="s">
         <v>173</v>
       </c>
       <c r="AV20" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="AX20" s="6" t="s">
+      <c r="AX20" s="4" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="50.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
         <v>21</v>
       </c>
@@ -2169,7 +1981,7 @@
       <c r="D21" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E21" s="1" t="n">
+      <c r="G21" s="1" t="n">
         <v>300</v>
       </c>
       <c r="Q21" s="0" t="n">
@@ -2187,18 +1999,10 @@
       <c r="W21" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="X21" s="1"/>
-      <c r="Y21" s="1"/>
-      <c r="Z21" s="0" t="n">
-        <v>15</v>
-      </c>
       <c r="AG21" s="1" t="n">
         <v>300</v>
       </c>
-      <c r="AT21" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AU21" s="5" t="s">
+      <c r="AU21" s="1" t="s">
         <v>180</v>
       </c>
       <c r="AV21" s="1" t="s">
@@ -2208,7 +2012,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="50.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
         <v>22</v>
       </c>
@@ -2221,7 +2025,7 @@
       <c r="D22" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E22" s="1" t="n">
+      <c r="G22" s="1" t="n">
         <v>320</v>
       </c>
       <c r="Q22" s="0" t="n">
@@ -2239,18 +2043,10 @@
       <c r="W22" s="1" t="n">
         <v>751</v>
       </c>
-      <c r="X22" s="1"/>
-      <c r="Y22" s="1"/>
-      <c r="Z22" s="0" t="n">
-        <v>15</v>
-      </c>
       <c r="AG22" s="1" t="n">
         <v>320</v>
       </c>
-      <c r="AT22" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AU22" s="5" t="s">
+      <c r="AU22" s="1" t="s">
         <v>185</v>
       </c>
       <c r="AV22" s="1" t="s">
@@ -2260,7 +2056,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="62.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
         <v>23</v>
       </c>
@@ -2270,10 +2066,10 @@
       <c r="C23" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="D23" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="E23" s="1" t="n">
+      <c r="D23" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G23" s="1" t="n">
         <v>195</v>
       </c>
       <c r="Q23" s="0" t="n">
@@ -2291,18 +2087,10 @@
       <c r="W23" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="X23" s="1"/>
-      <c r="Y23" s="1"/>
-      <c r="Z23" s="0" t="n">
-        <v>15</v>
-      </c>
       <c r="AG23" s="1" t="n">
         <v>195</v>
       </c>
-      <c r="AT23" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AU23" s="5" t="s">
+      <c r="AU23" s="1" t="s">
         <v>190</v>
       </c>
       <c r="AV23" s="1" t="s">
@@ -2312,7 +2100,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
         <v>24</v>
       </c>
@@ -2325,7 +2113,7 @@
       <c r="D24" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E24" s="1"/>
+      <c r="G24" s="1"/>
       <c r="Q24" s="0" t="n">
         <v>9786070283734</v>
       </c>
@@ -2341,16 +2129,8 @@
       <c r="W24" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="X24" s="1"/>
-      <c r="Y24" s="1"/>
-      <c r="Z24" s="0" t="n">
-        <v>15</v>
-      </c>
       <c r="AG24" s="1"/>
-      <c r="AT24" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AU24" s="5" t="s">
+      <c r="AU24" s="1" t="s">
         <v>198</v>
       </c>
       <c r="AV24" s="1" t="s">
@@ -2360,7 +2140,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="62.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="n">
         <v>25</v>
       </c>
@@ -2373,7 +2153,7 @@
       <c r="D25" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E25" s="1"/>
+      <c r="G25" s="1"/>
       <c r="Q25" s="0" t="n">
         <v>9786072001213</v>
       </c>
@@ -2389,16 +2169,8 @@
       <c r="W25" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="X25" s="1"/>
-      <c r="Y25" s="1"/>
-      <c r="Z25" s="0" t="n">
-        <v>15</v>
-      </c>
       <c r="AG25" s="1"/>
-      <c r="AT25" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AU25" s="5" t="s">
+      <c r="AU25" s="1" t="s">
         <v>203</v>
       </c>
       <c r="AV25" s="1" t="s">
@@ -2408,7 +2180,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="50.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="n">
         <v>26</v>
       </c>
@@ -2421,7 +2193,7 @@
       <c r="D26" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E26" s="1" t="n">
+      <c r="G26" s="1" t="n">
         <v>400</v>
       </c>
       <c r="Q26" s="0" t="n">
@@ -2439,18 +2211,10 @@
       <c r="W26" s="1" t="n">
         <v>869</v>
       </c>
-      <c r="X26" s="1"/>
-      <c r="Y26" s="1"/>
-      <c r="Z26" s="0" t="n">
-        <v>15</v>
-      </c>
       <c r="AG26" s="1" t="n">
         <v>400</v>
       </c>
-      <c r="AT26" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AU26" s="5" t="s">
+      <c r="AU26" s="1" t="s">
         <v>209</v>
       </c>
       <c r="AV26" s="1" t="s">
@@ -2460,7 +2224,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="147.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="172.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="n">
         <v>27</v>
       </c>
@@ -2473,7 +2237,7 @@
       <c r="D27" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E27" s="1" t="n">
+      <c r="G27" s="1" t="n">
         <v>260</v>
       </c>
       <c r="Q27" s="0" t="n">
@@ -2491,18 +2255,10 @@
       <c r="W27" s="1" t="n">
         <v>380</v>
       </c>
-      <c r="X27" s="1"/>
-      <c r="Y27" s="1"/>
-      <c r="Z27" s="0" t="n">
-        <v>15</v>
-      </c>
       <c r="AG27" s="1" t="n">
         <v>260</v>
       </c>
-      <c r="AT27" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AU27" s="5" t="s">
+      <c r="AU27" s="1" t="s">
         <v>214</v>
       </c>
       <c r="AV27" s="1" t="s">
@@ -2512,7 +2268,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="38.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="n">
         <v>28</v>
       </c>
@@ -2525,7 +2281,7 @@
       <c r="D28" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E28" s="1" t="n">
+      <c r="G28" s="1" t="n">
         <v>180</v>
       </c>
       <c r="Q28" s="0" t="n">
@@ -2543,18 +2299,10 @@
       <c r="W28" s="1" t="n">
         <v>444</v>
       </c>
-      <c r="X28" s="1"/>
-      <c r="Y28" s="1"/>
-      <c r="Z28" s="0" t="n">
-        <v>15</v>
-      </c>
       <c r="AG28" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="AT28" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AU28" s="5" t="s">
+      <c r="AU28" s="1" t="s">
         <v>219</v>
       </c>
       <c r="AV28" s="1" t="s">
@@ -2564,7 +2312,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="62.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="n">
         <v>28</v>
       </c>
@@ -2577,7 +2325,7 @@
       <c r="D29" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E29" s="1"/>
+      <c r="G29" s="1"/>
       <c r="Q29" s="2"/>
       <c r="T29" s="1" t="n">
         <v>11</v>
@@ -2591,16 +2339,8 @@
       <c r="W29" s="1" t="n">
         <v>153</v>
       </c>
-      <c r="X29" s="1"/>
-      <c r="Y29" s="1"/>
-      <c r="Z29" s="0" t="n">
-        <v>15</v>
-      </c>
       <c r="AG29" s="1"/>
-      <c r="AT29" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AU29" s="5" t="s">
+      <c r="AU29" s="1" t="s">
         <v>223</v>
       </c>
       <c r="AV29" s="1" t="s">
@@ -2610,7 +2350,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="n">
         <v>30</v>
       </c>
@@ -2623,7 +2363,7 @@
       <c r="D30" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E30" s="1" t="n">
+      <c r="G30" s="1" t="n">
         <v>180</v>
       </c>
       <c r="Q30" s="2"/>
@@ -2639,18 +2379,10 @@
       <c r="W30" s="1" t="n">
         <v>444</v>
       </c>
-      <c r="X30" s="1"/>
-      <c r="Y30" s="1"/>
-      <c r="Z30" s="0" t="n">
-        <v>15</v>
-      </c>
       <c r="AG30" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="AT30" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AU30" s="5" t="s">
+      <c r="AU30" s="1" t="s">
         <v>227</v>
       </c>
       <c r="AV30" s="1" t="s">

</xml_diff>